<commit_message>
Add Arabic guidance rows to all Excel template files
Co-authored-by: MohabTohamy <167503329+MohabTohamy@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/قالب-fwd.xlsx
+++ b/قالب-fwd.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FWD" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="FWD" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,13 +25,24 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i val="1"/>
+      <color rgb="00666666"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F0F0F0"/>
+        <bgColor rgb="00F0F0F0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +57,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,18 +452,35 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>أدخل رمز القطاع/المقطع (مثال: 0120010601014020001)</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>أدخل رقم المسار (L1, L2, إلخ)</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>أدخل قراءة جهاز FWD بالميكرون (مثال: 310.5)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>0120010601014020001</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>L1</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C3" t="n">
         <v>310.5</v>
       </c>
     </row>

</xml_diff>